<commit_message>
Screen Resolution in Settings
</commit_message>
<xml_diff>
--- a/Assets/Game Data/LocalizationData.xlsx
+++ b/Assets/Game Data/LocalizationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitRepository\3D_RPG\Assets\Game Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3939D0DE-43E6-4B34-9482-46D873700B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F100397-03AE-489F-869A-EB6993D452A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6135" yWindow="1980" windowWidth="20070" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,6 +281,18 @@
   </si>
   <si>
     <t>請輸入存檔名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_screen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全屏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FULL SCREEN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -609,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -872,6 +884,20 @@
         <v>64</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>